<commit_message>
Cambio en archivo excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/RetoTecnico.xlsx
+++ b/src/test/resources/data/RetoTecnico.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>inputDesdeViaje</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t>Santa Marta</t>
-  </si>
-  <si>
-    <t>Cali</t>
-  </si>
-  <si>
-    <t>Cartagena</t>
   </si>
 </sst>
 </file>
@@ -387,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,23 +431,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>